<commit_message>
change file list bank tujuan disbursement
</commit_message>
<xml_diff>
--- a/src/assets/files/Daftar Bank Tujuan Disbursement-PT. Ezeelink Indonesia.xlsx
+++ b/src/assets/files/Daftar Bank Tujuan Disbursement-PT. Ezeelink Indonesia.xlsx
@@ -1,11 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ezeelink\PaymentGatewayPortalGit\PaymentGatewayPortal\src\assets\files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6B93A09-BFDA-40D8-861E-92EE146735E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7070"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daftar Bank Tujuan" sheetId="1" r:id="rId1"/>
@@ -15,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="195">
   <si>
     <t>Daftar Bank Tujuan Disbursement - PT. Ezeelink Indonesia</t>
   </si>
@@ -475,9 +481,6 @@
     <t>GANESHA</t>
   </si>
   <si>
-    <t>KUSTODIAN SENTRAL EFEK INDONESIA</t>
-  </si>
-  <si>
     <t>008</t>
   </si>
   <si>
@@ -613,14 +616,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -647,148 +644,10 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -807,194 +666,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="21">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1134,251 +807,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1392,6 +823,33 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1428,87 +886,15 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FFFFC7CE"/>
@@ -1516,9 +902,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FFFFC7CE"/>
@@ -1530,6 +913,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1787,1150 +1173,1140 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:C105"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="G76" sqref="G76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.72727272727273" style="1"/>
-    <col min="2" max="2" width="10.5454545454545" style="2" customWidth="1"/>
-    <col min="3" max="3" width="63.9090909090909" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.72727272727273" style="1"/>
+    <col min="1" max="1" width="8.77734375" style="1"/>
+    <col min="2" max="2" width="10.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="63.88671875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" ht="14.55" customHeight="1">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="17"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="20"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="20"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="20"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="20"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="23"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="17">
+      <c r="A10" s="5">
         <v>1</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="17">
+      <c r="A11" s="5">
         <v>2</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="17">
+      <c r="A12" s="5">
         <v>3</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="17">
+      <c r="A13" s="5">
         <v>4</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="17">
+      <c r="A14" s="5">
         <v>5</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="17">
+      <c r="A15" s="5">
         <v>6</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="17">
+      <c r="A16" s="5">
         <v>7</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="17">
+      <c r="A17" s="5">
         <v>8</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="17">
+      <c r="A18" s="5">
         <v>9</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="17">
+      <c r="A19" s="5">
         <v>10</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="17">
+      <c r="A20" s="5">
         <v>11</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="17">
+      <c r="A21" s="5">
         <v>12</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="17">
+      <c r="A22" s="5">
         <v>13</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="10" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="17">
+      <c r="A23" s="5">
         <v>14</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="17">
+      <c r="A24" s="5">
         <v>15</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="9" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="17">
+      <c r="A25" s="5">
         <v>16</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="9" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="17">
+      <c r="A26" s="5">
         <v>17</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="11" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="17">
+      <c r="A27" s="5">
         <v>18</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="9" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="17">
+      <c r="A28" s="5">
         <v>19</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="17">
+      <c r="A29" s="5">
         <v>20</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C29" s="9" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="17">
+      <c r="A30" s="5">
         <v>21</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="9" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="17">
+      <c r="A31" s="5">
         <v>22</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="9" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="17">
+      <c r="A32" s="5">
         <v>23</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="9" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="17">
+      <c r="A33" s="5">
         <v>24</v>
       </c>
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="C33" s="9" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="17">
+      <c r="A34" s="5">
         <v>25</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="C34" s="10" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="17">
+      <c r="A35" s="5">
         <v>26</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="C35" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="17">
+      <c r="A36" s="5">
         <v>27</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C36" s="21" t="s">
+      <c r="C36" s="9" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="17">
+      <c r="A37" s="5">
         <v>28</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C37" s="21" t="s">
+      <c r="C37" s="9" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="17">
+      <c r="A38" s="5">
         <v>29</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C38" s="22" t="s">
+      <c r="C38" s="10" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="17">
+      <c r="A39" s="5">
         <v>30</v>
       </c>
-      <c r="B39" s="20" t="s">
+      <c r="B39" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C39" s="21" t="s">
+      <c r="C39" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="17">
+      <c r="A40" s="5">
         <v>31</v>
       </c>
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="21" t="s">
+      <c r="C40" s="9" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="17">
+      <c r="A41" s="5">
         <v>32</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C41" s="22" t="s">
+      <c r="C41" s="10" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="17">
+      <c r="A42" s="5">
         <v>33</v>
       </c>
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C42" s="21" t="s">
+      <c r="C42" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="17">
+      <c r="A43" s="5">
         <v>34</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C43" s="22" t="s">
+      <c r="C43" s="10" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="17">
+      <c r="A44" s="5">
         <v>35</v>
       </c>
-      <c r="B44" s="20" t="s">
+      <c r="B44" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C44" s="21" t="s">
+      <c r="C44" s="9" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="17">
+      <c r="A45" s="5">
         <v>36</v>
       </c>
-      <c r="B45" s="20" t="s">
+      <c r="B45" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C45" s="22" t="s">
+      <c r="C45" s="10" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="17">
+      <c r="A46" s="5">
         <v>37</v>
       </c>
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C46" s="22" t="s">
+      <c r="C46" s="10" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="17">
+      <c r="A47" s="5">
         <v>38</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C47" s="22" t="s">
+      <c r="C47" s="10" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="17">
+      <c r="A48" s="5">
         <v>39</v>
       </c>
-      <c r="B48" s="20" t="s">
+      <c r="B48" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C48" s="22" t="s">
+      <c r="C48" s="10" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="17">
+      <c r="A49" s="5">
         <v>40</v>
       </c>
-      <c r="B49" s="20" t="s">
+      <c r="B49" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C49" s="22" t="s">
+      <c r="C49" s="10" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="17">
+      <c r="A50" s="5">
         <v>41</v>
       </c>
-      <c r="B50" s="20" t="s">
+      <c r="B50" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C50" s="21" t="s">
+      <c r="C50" s="9" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="17">
+      <c r="A51" s="5">
         <v>42</v>
       </c>
-      <c r="B51" s="20" t="s">
+      <c r="B51" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C51" s="21" t="s">
+      <c r="C51" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="17">
+      <c r="A52" s="5">
         <v>43</v>
       </c>
-      <c r="B52" s="20" t="s">
+      <c r="B52" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C52" s="21" t="s">
+      <c r="C52" s="9" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="17">
+      <c r="A53" s="5">
         <v>44</v>
       </c>
-      <c r="B53" s="20" t="s">
+      <c r="B53" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C53" s="21" t="s">
+      <c r="C53" s="9" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="17">
+      <c r="A54" s="5">
         <v>45</v>
       </c>
-      <c r="B54" s="20" t="s">
+      <c r="B54" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C54" s="21" t="s">
+      <c r="C54" s="9" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="17">
+      <c r="A55" s="5">
         <v>46</v>
       </c>
-      <c r="B55" s="20" t="s">
+      <c r="B55" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C55" s="22" t="s">
+      <c r="C55" s="10" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="17">
+      <c r="A56" s="5">
         <v>47</v>
       </c>
-      <c r="B56" s="20" t="s">
+      <c r="B56" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C56" s="22" t="s">
+      <c r="C56" s="10" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="17">
+      <c r="A57" s="5">
         <v>48</v>
       </c>
-      <c r="B57" s="20" t="s">
+      <c r="B57" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C57" s="22" t="s">
+      <c r="C57" s="10" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="17">
+      <c r="A58" s="5">
         <v>49</v>
       </c>
-      <c r="B58" s="20" t="s">
+      <c r="B58" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C58" s="21" t="s">
+      <c r="C58" s="9" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="17">
+      <c r="A59" s="5">
         <v>50</v>
       </c>
-      <c r="B59" s="20" t="s">
+      <c r="B59" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C59" s="21" t="s">
+      <c r="C59" s="9" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="17">
+      <c r="A60" s="5">
         <v>51</v>
       </c>
-      <c r="B60" s="20" t="s">
+      <c r="B60" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C60" s="21" t="s">
+      <c r="C60" s="9" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="17">
+      <c r="A61" s="5">
         <v>52</v>
       </c>
-      <c r="B61" s="20" t="s">
+      <c r="B61" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C61" s="21" t="s">
+      <c r="C61" s="9" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="17">
+      <c r="A62" s="5">
         <v>53</v>
       </c>
-      <c r="B62" s="20" t="s">
+      <c r="B62" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C62" s="21" t="s">
+      <c r="C62" s="9" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="17">
+      <c r="A63" s="5">
         <v>54</v>
       </c>
-      <c r="B63" s="20" t="s">
+      <c r="B63" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="C63" s="21" t="s">
+      <c r="C63" s="9" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="17">
+      <c r="A64" s="5">
         <v>55</v>
       </c>
-      <c r="B64" s="20" t="s">
+      <c r="B64" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C64" s="21" t="s">
+      <c r="C64" s="9" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="17">
+      <c r="A65" s="5">
         <v>56</v>
       </c>
-      <c r="B65" s="20" t="s">
+      <c r="B65" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C65" s="21" t="s">
+      <c r="C65" s="9" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="17">
+      <c r="A66" s="5">
         <v>57</v>
       </c>
-      <c r="B66" s="20" t="s">
+      <c r="B66" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="C66" s="22" t="s">
+      <c r="C66" s="10" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="17">
+      <c r="A67" s="5">
         <v>58</v>
       </c>
-      <c r="B67" s="20" t="s">
+      <c r="B67" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C67" s="21" t="s">
+      <c r="C67" s="9" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="17">
+      <c r="A68" s="5">
         <v>59</v>
       </c>
-      <c r="B68" s="20" t="s">
+      <c r="B68" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="C68" s="22" t="s">
+      <c r="C68" s="10" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="17">
+      <c r="A69" s="5">
         <v>60</v>
       </c>
-      <c r="B69" s="20" t="s">
+      <c r="B69" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="C69" s="21" t="s">
+      <c r="C69" s="9" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="17">
+      <c r="A70" s="5">
         <v>61</v>
       </c>
-      <c r="B70" s="20" t="s">
+      <c r="B70" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C70" s="21" t="s">
+      <c r="C70" s="9" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="17">
+      <c r="A71" s="5">
         <v>62</v>
       </c>
-      <c r="B71" s="20" t="s">
+      <c r="B71" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="C71" s="21" t="s">
+      <c r="C71" s="9" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="17">
+      <c r="A72" s="5">
         <v>63</v>
       </c>
-      <c r="B72" s="20" t="s">
+      <c r="B72" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="C72" s="21" t="s">
+      <c r="C72" s="9" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="17">
+      <c r="A73" s="5">
         <v>64</v>
       </c>
-      <c r="B73" s="20" t="s">
+      <c r="B73" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="C73" s="21" t="s">
+      <c r="C73" s="9" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="17">
+      <c r="A74" s="5">
         <v>65</v>
       </c>
-      <c r="B74" s="20" t="s">
+      <c r="B74" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="C74" s="21" t="s">
+      <c r="C74" s="9" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="17">
+      <c r="A75" s="5">
         <v>66</v>
       </c>
-      <c r="B75" s="20" t="s">
+      <c r="B75" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="C75" s="21" t="s">
+      <c r="C75" s="9" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="17">
+      <c r="A76" s="5">
         <v>67</v>
       </c>
-      <c r="B76" s="20" t="s">
+      <c r="B76" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="C76" s="21" t="s">
+      <c r="C76" s="9" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="17">
+      <c r="A77" s="5">
         <v>68</v>
       </c>
-      <c r="B77" s="20" t="s">
+      <c r="B77" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="C77" s="22" t="s">
+      <c r="C77" s="10" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="17">
+      <c r="A78" s="5">
         <v>69</v>
       </c>
-      <c r="B78" s="20" t="s">
+      <c r="B78" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="C78" s="22" t="s">
+      <c r="C78" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" s="17">
+      <c r="A79" s="5">
         <v>70</v>
       </c>
-      <c r="B79" s="20" t="s">
+      <c r="B79" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="C79" s="22" t="s">
+      <c r="C79" s="10" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" s="17">
+      <c r="A80" s="5">
         <v>71</v>
       </c>
-      <c r="B80" s="20" t="s">
+      <c r="B80" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="C80" s="22" t="s">
+      <c r="C80" s="10" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" s="17">
+      <c r="A81" s="5">
         <v>72</v>
       </c>
-      <c r="B81" s="20" t="s">
+      <c r="B81" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="C81" s="22" t="s">
+      <c r="C81" s="10" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="17">
+      <c r="A82" s="5">
         <v>73</v>
       </c>
-      <c r="B82" s="20" t="s">
+      <c r="B82" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="C82" s="22" t="s">
+      <c r="C82" s="10" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="17">
+      <c r="A83" s="5">
         <v>74</v>
       </c>
-      <c r="B83" s="20"/>
-      <c r="C83" s="21" t="s">
+      <c r="B83" s="8" t="s">
         <v>151</v>
       </c>
+      <c r="C83" s="10" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" s="17">
+      <c r="A84" s="5">
         <v>75</v>
       </c>
-      <c r="B84" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="C84" s="22" t="s">
+      <c r="B84" s="8" t="s">
         <v>153</v>
       </c>
+      <c r="C84" s="10" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="17">
+      <c r="A85" s="5">
         <v>76</v>
       </c>
-      <c r="B85" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="C85" s="22" t="s">
+      <c r="B85" s="8" t="s">
         <v>155</v>
       </c>
+      <c r="C85" s="9" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="17">
+      <c r="A86" s="5">
         <v>77</v>
       </c>
-      <c r="B86" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="C86" s="21" t="s">
+      <c r="B86" s="8" t="s">
         <v>157</v>
       </c>
+      <c r="C86" s="10" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="17">
+      <c r="A87" s="5">
         <v>78</v>
       </c>
-      <c r="B87" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="C87" s="22" t="s">
+      <c r="B87" s="8" t="s">
         <v>159</v>
       </c>
+      <c r="C87" s="10" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" s="17">
+      <c r="A88" s="5">
         <v>79</v>
       </c>
-      <c r="B88" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="C88" s="22" t="s">
+      <c r="B88" s="8" t="s">
         <v>161</v>
       </c>
+      <c r="C88" s="9" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="17">
+      <c r="A89" s="5">
         <v>80</v>
       </c>
-      <c r="B89" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="C89" s="21" t="s">
+      <c r="B89" s="8" t="s">
         <v>163</v>
       </c>
+      <c r="C89" s="9" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" s="17">
+      <c r="A90" s="5">
         <v>81</v>
       </c>
-      <c r="B90" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="C90" s="21" t="s">
+      <c r="B90" s="8" t="s">
         <v>165</v>
       </c>
+      <c r="C90" s="10" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="17">
+      <c r="A91" s="5">
         <v>82</v>
       </c>
-      <c r="B91" s="20" t="s">
-        <v>166</v>
-      </c>
-      <c r="C91" s="22" t="s">
+      <c r="B91" s="8" t="s">
         <v>167</v>
       </c>
+      <c r="C91" s="10" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92" s="17">
+      <c r="A92" s="5">
         <v>83</v>
       </c>
-      <c r="B92" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="C92" s="22" t="s">
+      <c r="B92" s="8" t="s">
         <v>169</v>
       </c>
+      <c r="C92" s="10" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" s="17">
+      <c r="A93" s="5">
         <v>84</v>
       </c>
-      <c r="B93" s="20" t="s">
-        <v>170</v>
-      </c>
-      <c r="C93" s="22" t="s">
+      <c r="B93" s="8" t="s">
         <v>171</v>
       </c>
+      <c r="C93" s="10" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" s="17">
+      <c r="A94" s="5">
         <v>85</v>
       </c>
-      <c r="B94" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="C94" s="22" t="s">
+      <c r="B94" s="8" t="s">
         <v>173</v>
       </c>
+      <c r="C94" s="10" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" s="17">
+      <c r="A95" s="5">
         <v>86</v>
       </c>
-      <c r="B95" s="20" t="s">
-        <v>174</v>
-      </c>
-      <c r="C95" s="22" t="s">
+      <c r="B95" s="8" t="s">
         <v>175</v>
       </c>
+      <c r="C95" s="10" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" s="17">
+      <c r="A96" s="5">
         <v>87</v>
       </c>
-      <c r="B96" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="C96" s="22" t="s">
+      <c r="B96" s="8" t="s">
         <v>177</v>
       </c>
+      <c r="C96" s="10" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="17">
+      <c r="A97" s="5">
         <v>88</v>
       </c>
-      <c r="B97" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="C97" s="22" t="s">
+      <c r="B97" s="8" t="s">
         <v>179</v>
       </c>
+      <c r="C97" s="10" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" s="17">
+      <c r="A98" s="5">
         <v>89</v>
       </c>
-      <c r="B98" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="C98" s="22" t="s">
+      <c r="B98" s="8" t="s">
         <v>181</v>
       </c>
+      <c r="C98" s="10" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="99" spans="1:3">
-      <c r="A99" s="17">
+      <c r="A99" s="5">
         <v>90</v>
       </c>
-      <c r="B99" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="C99" s="22" t="s">
+      <c r="B99" s="8" t="s">
         <v>183</v>
       </c>
+      <c r="C99" s="10" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="100" spans="1:3">
-      <c r="A100" s="17">
+      <c r="A100" s="5">
         <v>91</v>
       </c>
-      <c r="B100" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="C100" s="22" t="s">
+      <c r="B100" s="8" t="s">
         <v>185</v>
       </c>
+      <c r="C100" s="9" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="101" spans="1:3">
-      <c r="A101" s="17">
+      <c r="A101" s="5">
         <v>92</v>
       </c>
-      <c r="B101" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="C101" s="21" t="s">
+      <c r="B101" s="8" t="s">
         <v>187</v>
       </c>
+      <c r="C101" s="10" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="102" spans="1:3">
-      <c r="A102" s="17">
+      <c r="A102" s="5">
         <v>93</v>
       </c>
-      <c r="B102" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="C102" s="22" t="s">
+      <c r="B102" s="8" t="s">
         <v>189</v>
       </c>
+      <c r="C102" s="10" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="103" spans="1:3">
-      <c r="A103" s="17">
+      <c r="A103" s="5">
         <v>94</v>
       </c>
-      <c r="B103" s="20" t="s">
-        <v>190</v>
-      </c>
-      <c r="C103" s="22" t="s">
+      <c r="B103" s="8" t="s">
         <v>191</v>
       </c>
+      <c r="C103" s="9" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="104" spans="1:3">
-      <c r="A104" s="17">
+      <c r="A104" s="5">
         <v>95</v>
       </c>
-      <c r="B104" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="C104" s="21" t="s">
+      <c r="B104" s="8" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="105" spans="1:3">
-      <c r="A105" s="17">
-        <v>96</v>
-      </c>
-      <c r="B105" s="20" t="s">
+      <c r="C104" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="C105" s="22" t="s">
-        <v>195</v>
-      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C111">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C110">
     <sortCondition ref="C1"/>
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C8"/>
   </mergeCells>
-  <conditionalFormatting sqref="B$1:B$1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:C61">
-    <cfRule type="duplicateValues" dxfId="1" priority="2" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2" stopIfTrue="1"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>